<commit_message>
Added 29C040 ROM component for controller-sequencer module
</commit_message>
<xml_diff>
--- a/Documentation/Instructions_T-States.xlsx
+++ b/Documentation/Instructions_T-States.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Projects\Active\TTL-Computer\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6787884C-4E96-4A6B-B264-11610FC141B3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32ADC23-57D7-428A-8898-4D6A22D098E4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9132" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="287">
   <si>
     <t>Opcode</t>
   </si>
@@ -4505,13 +4505,37 @@
   </si>
   <si>
     <t>[00000000][00000000]</t>
+  </si>
+  <si>
+    <t>Decoding ROM (29C040) has 19 address bits</t>
+  </si>
+  <si>
+    <t>6 bit instruction</t>
+  </si>
+  <si>
+    <t>4 bit t-state</t>
+  </si>
+  <si>
+    <t>3 bit group (We need 6 groups of 8 bits for the control word (6x8 bits = 48 bits control word)</t>
+  </si>
+  <si>
+    <t>5 bit flags (There are 5 flags)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">= 18 bits address </t>
+  </si>
+  <si>
+    <t>[0][000][00000][000000][0000]</t>
+  </si>
+  <si>
+    <t>[unused][group][flags][instruction][t-state]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4625,6 +4649,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -4709,7 +4750,6 @@
   </cellStyleXfs>
   <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4718,13 +4758,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4742,7 +4781,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4758,7 +4797,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="45"/>
     </xf>
@@ -4791,6 +4829,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5107,650 +5148,650 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J34"/>
+    <sheetView topLeftCell="F31" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" style="3" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="7.109375" style="3" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" style="3" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="16" style="3" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="40.33203125" style="3" hidden="1" customWidth="1"/>
-    <col min="6" max="9" width="9.109375" style="3"/>
-    <col min="10" max="10" width="24.88671875" style="3" customWidth="1"/>
-    <col min="11" max="11" width="60.5546875" style="3" customWidth="1"/>
-    <col min="12" max="16384" width="9.109375" style="3"/>
+    <col min="1" max="1" width="9.5546875" style="2" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="7.109375" style="2" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" style="2" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="16" style="2" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="40.33203125" style="2" hidden="1" customWidth="1"/>
+    <col min="6" max="9" width="9.109375" style="2"/>
+    <col min="10" max="10" width="24.88671875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="60.5546875" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="K1" s="2"/>
+      <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="2" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="2" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="K5" s="2" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="K6" s="2" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="K7" s="2" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="K8" s="2" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="J9" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="K9" s="2" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="J10" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="K10" s="3" t="s">
+      <c r="K10" s="2" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J11" s="3" t="s">
+      <c r="J11" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="K11" s="3" t="s">
+      <c r="K11" s="2" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="J12" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="K12" s="3" t="s">
+      <c r="K12" s="2" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J13" s="3" t="s">
+      <c r="J13" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="K13" s="3" t="s">
+      <c r="K13" s="2" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J14" s="3" t="s">
+      <c r="J14" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="K14" s="3" t="s">
+      <c r="K14" s="2" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="3" t="s">
+      <c r="J15" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="K15" s="3" t="s">
+      <c r="K15" s="2" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J16" s="3" t="s">
+      <c r="J16" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="K16" s="3" t="s">
+      <c r="K16" s="2" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="3" t="s">
+      <c r="J17" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="K17" s="3" t="s">
+      <c r="K17" s="2" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="J18" s="3" t="s">
+      <c r="J18" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="K18" s="3" t="s">
+      <c r="K18" s="2" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="J19" s="3" t="s">
+      <c r="J19" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="K19" s="3" t="s">
+      <c r="K19" s="2" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="J20" s="3" t="s">
+      <c r="J20" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="K20" s="3" t="s">
+      <c r="K20" s="2" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="J21" s="3" t="s">
+      <c r="J21" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="K21" s="3" t="s">
+      <c r="K21" s="2" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="J22" s="3" t="s">
+      <c r="J22" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="K22" s="3" t="s">
+      <c r="K22" s="2" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J23" s="3" t="s">
+      <c r="J23" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="K23" s="3" t="s">
+      <c r="K23" s="2" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J24" s="3" t="s">
+      <c r="J24" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="K24" s="3" t="s">
+      <c r="K24" s="2" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J25" s="3" t="s">
+      <c r="J25" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="K25" s="3" t="s">
+      <c r="K25" s="2" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F26" s="38"/>
-      <c r="J26" s="3" t="s">
+      <c r="F26" s="35"/>
+      <c r="J26" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="K26" s="3" t="s">
+      <c r="K26" s="2" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="J27" s="3" t="s">
+      <c r="J27" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="K27" s="3" t="s">
+      <c r="K27" s="2" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E28" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F28" s="5"/>
-      <c r="J28" s="3" t="s">
+      <c r="F28" s="4"/>
+      <c r="J28" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="K28" s="3" t="s">
+      <c r="K28" s="2" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E29" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="J29" s="3" t="s">
+      <c r="J29" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="K29" s="3" t="s">
+      <c r="K29" s="2" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E30" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="J30" s="3" t="s">
+      <c r="J30" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="K30" s="3" t="s">
+      <c r="K30" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="J31" s="3" t="s">
+      <c r="J31" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="K31" s="3" t="s">
+      <c r="K31" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E32" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="J32" s="3" t="s">
+      <c r="J32" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="K32" s="3" t="s">
+      <c r="K32" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="J33" s="3" t="s">
+      <c r="J33" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="K33" s="3" t="s">
+      <c r="K33" s="2" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E34" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="J34" s="3" t="s">
+      <c r="J34" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="K34" s="3" t="s">
+      <c r="K34" s="2" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E35" s="2" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E36" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E37" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="E38" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E39" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="39" t="s">
+      <c r="A40" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="B40" s="40"/>
-      <c r="C40" s="40" t="s">
+      <c r="B40" s="37"/>
+      <c r="C40" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="D40" s="40"/>
-      <c r="E40" s="40" t="s">
+      <c r="D40" s="37"/>
+      <c r="E40" s="37" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="39" t="s">
+      <c r="A41" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="B41" s="40"/>
-      <c r="C41" s="40" t="s">
+      <c r="B41" s="37"/>
+      <c r="C41" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="D41" s="40"/>
-      <c r="E41" s="40" t="s">
+      <c r="D41" s="37"/>
+      <c r="E41" s="37" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="B42" s="40"/>
-      <c r="C42" s="40" t="s">
+      <c r="B42" s="37"/>
+      <c r="C42" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="D42" s="40"/>
-      <c r="E42" s="40" t="s">
+      <c r="D42" s="37"/>
+      <c r="E42" s="37" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="E43" s="2" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="E44" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="E45" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="E46" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E47" s="3" t="s">
+      <c r="E47" s="2" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
+      <c r="A48" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E48" s="3" t="s">
+      <c r="E48" s="2" t="s">
         <v>75</v>
       </c>
     </row>
@@ -5771,185 +5812,185 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.4">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.4">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.4">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.4">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.4">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.4">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.4">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.4">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="5" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.4">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.4">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.4">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.4">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.4">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.4">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.4">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.4">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="18" x14ac:dyDescent="0.4">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="6"/>
+      <c r="A18" s="5"/>
     </row>
     <row r="19" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="6"/>
+      <c r="A19" s="5"/>
     </row>
     <row r="20" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="6"/>
+      <c r="A20" s="5"/>
     </row>
     <row r="21" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="6"/>
+      <c r="A21" s="5"/>
     </row>
     <row r="22" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="6"/>
+      <c r="A22" s="5"/>
     </row>
     <row r="23" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="6"/>
+      <c r="A23" s="5"/>
     </row>
     <row r="24" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="6"/>
+      <c r="A24" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5967,1686 +6008,1684 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4" style="3" customWidth="1"/>
-    <col min="2" max="2" width="32" style="3" customWidth="1"/>
-    <col min="3" max="3" width="5.109375" style="19" customWidth="1"/>
-    <col min="4" max="4" width="5.109375" style="13" customWidth="1"/>
-    <col min="5" max="5" width="5.109375" style="19" customWidth="1"/>
-    <col min="6" max="6" width="5.109375" style="13" customWidth="1"/>
-    <col min="7" max="7" width="5.109375" style="19" customWidth="1"/>
-    <col min="8" max="8" width="5.109375" style="13" customWidth="1"/>
-    <col min="9" max="9" width="5.109375" style="19" customWidth="1"/>
-    <col min="10" max="10" width="5.109375" style="13" customWidth="1"/>
-    <col min="11" max="11" width="5.109375" style="19" customWidth="1"/>
-    <col min="12" max="12" width="5.109375" style="13" customWidth="1"/>
-    <col min="13" max="13" width="5.109375" style="19" customWidth="1"/>
-    <col min="14" max="14" width="5.109375" style="13" customWidth="1"/>
-    <col min="15" max="15" width="5.109375" style="19" customWidth="1"/>
-    <col min="16" max="16" width="5.109375" style="13" customWidth="1"/>
-    <col min="17" max="17" width="5.109375" style="19" customWidth="1"/>
-    <col min="18" max="18" width="5.109375" style="13" customWidth="1"/>
-    <col min="19" max="19" width="5.109375" style="19" customWidth="1"/>
-    <col min="20" max="20" width="5.109375" style="13" customWidth="1"/>
-    <col min="21" max="21" width="5.109375" style="19" customWidth="1"/>
-    <col min="22" max="22" width="5.109375" style="13" customWidth="1"/>
-    <col min="23" max="23" width="5.109375" style="19" customWidth="1"/>
-    <col min="24" max="24" width="5.109375" style="13" customWidth="1"/>
-    <col min="25" max="25" width="5.109375" style="19" customWidth="1"/>
-    <col min="26" max="26" width="5.109375" style="13" customWidth="1"/>
-    <col min="27" max="27" width="5.109375" style="19" customWidth="1"/>
-    <col min="28" max="28" width="5.109375" style="13" customWidth="1"/>
-    <col min="29" max="29" width="5.109375" style="19" customWidth="1"/>
-    <col min="30" max="30" width="5.109375" style="13" customWidth="1"/>
-    <col min="31" max="31" width="5.109375" style="19" customWidth="1"/>
-    <col min="32" max="32" width="5.109375" style="13" customWidth="1"/>
-    <col min="33" max="33" width="5.109375" style="19" customWidth="1"/>
-    <col min="34" max="34" width="5.109375" style="13" customWidth="1"/>
-    <col min="35" max="35" width="5.109375" style="19" customWidth="1"/>
-    <col min="36" max="36" width="5.109375" style="13" customWidth="1"/>
-    <col min="37" max="37" width="5.109375" style="19" customWidth="1"/>
-    <col min="38" max="16384" width="9.109375" style="3"/>
+    <col min="1" max="1" width="4" style="2" customWidth="1"/>
+    <col min="2" max="2" width="32" style="2" customWidth="1"/>
+    <col min="3" max="3" width="5.109375" style="17" customWidth="1"/>
+    <col min="4" max="4" width="5.109375" style="11" customWidth="1"/>
+    <col min="5" max="5" width="5.109375" style="17" customWidth="1"/>
+    <col min="6" max="6" width="5.109375" style="11" customWidth="1"/>
+    <col min="7" max="7" width="5.109375" style="17" customWidth="1"/>
+    <col min="8" max="8" width="5.109375" style="11" customWidth="1"/>
+    <col min="9" max="9" width="5.109375" style="17" customWidth="1"/>
+    <col min="10" max="10" width="5.109375" style="11" customWidth="1"/>
+    <col min="11" max="11" width="5.109375" style="17" customWidth="1"/>
+    <col min="12" max="12" width="5.109375" style="11" customWidth="1"/>
+    <col min="13" max="13" width="5.109375" style="17" customWidth="1"/>
+    <col min="14" max="14" width="5.109375" style="11" customWidth="1"/>
+    <col min="15" max="15" width="5.109375" style="17" customWidth="1"/>
+    <col min="16" max="16" width="5.109375" style="11" customWidth="1"/>
+    <col min="17" max="17" width="5.109375" style="17" customWidth="1"/>
+    <col min="18" max="18" width="5.109375" style="11" customWidth="1"/>
+    <col min="19" max="19" width="5.109375" style="17" customWidth="1"/>
+    <col min="20" max="20" width="5.109375" style="11" customWidth="1"/>
+    <col min="21" max="21" width="5.109375" style="17" customWidth="1"/>
+    <col min="22" max="22" width="5.109375" style="11" customWidth="1"/>
+    <col min="23" max="23" width="5.109375" style="17" customWidth="1"/>
+    <col min="24" max="24" width="5.109375" style="11" customWidth="1"/>
+    <col min="25" max="25" width="5.109375" style="17" customWidth="1"/>
+    <col min="26" max="26" width="5.109375" style="11" customWidth="1"/>
+    <col min="27" max="27" width="5.109375" style="17" customWidth="1"/>
+    <col min="28" max="28" width="5.109375" style="11" customWidth="1"/>
+    <col min="29" max="29" width="5.109375" style="17" customWidth="1"/>
+    <col min="30" max="30" width="5.109375" style="11" customWidth="1"/>
+    <col min="31" max="31" width="5.109375" style="17" customWidth="1"/>
+    <col min="32" max="32" width="5.109375" style="11" customWidth="1"/>
+    <col min="33" max="33" width="5.109375" style="17" customWidth="1"/>
+    <col min="34" max="34" width="5.109375" style="11" customWidth="1"/>
+    <col min="35" max="35" width="5.109375" style="17" customWidth="1"/>
+    <col min="36" max="36" width="5.109375" style="11" customWidth="1"/>
+    <col min="37" max="37" width="5.109375" style="17" customWidth="1"/>
+    <col min="38" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="1" customFormat="1" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="10"/>
-      <c r="B1" s="10"/>
-      <c r="C1" s="27" t="s">
+    <row r="1" spans="1:38" customFormat="1" ht="46.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="H1" s="25" t="s">
         <v>140</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="J1" s="28" t="s">
+      <c r="J1" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="K1" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="L1" s="28" t="s">
+      <c r="L1" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="M1" s="27" t="s">
+      <c r="M1" s="24" t="s">
         <v>145</v>
       </c>
-      <c r="N1" s="28" t="s">
+      <c r="N1" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="O1" s="27" t="s">
+      <c r="O1" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="P1" s="28" t="s">
+      <c r="P1" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="Q1" s="27" t="s">
+      <c r="Q1" s="24" t="s">
         <v>148</v>
       </c>
-      <c r="R1" s="28" t="s">
+      <c r="R1" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="S1" s="27" t="s">
+      <c r="S1" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="T1" s="28" t="s">
+      <c r="T1" s="25" t="s">
         <v>151</v>
       </c>
-      <c r="U1" s="27" t="s">
+      <c r="U1" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="V1" s="28" t="s">
+      <c r="V1" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="W1" s="27" t="s">
+      <c r="W1" s="24" t="s">
         <v>154</v>
       </c>
-      <c r="X1" s="28" t="s">
+      <c r="X1" s="25" t="s">
         <v>155</v>
       </c>
-      <c r="Y1" s="27" t="s">
+      <c r="Y1" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="Z1" s="28" t="s">
+      <c r="Z1" s="25" t="s">
         <v>157</v>
       </c>
-      <c r="AA1" s="27" t="s">
+      <c r="AA1" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="AB1" s="28" t="s">
+      <c r="AB1" s="25" t="s">
         <v>159</v>
       </c>
-      <c r="AC1" s="27" t="s">
+      <c r="AC1" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="AD1" s="28" t="s">
+      <c r="AD1" s="25" t="s">
         <v>161</v>
       </c>
-      <c r="AE1" s="27" t="s">
+      <c r="AE1" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="AF1" s="28" t="s">
+      <c r="AF1" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="AG1" s="27" t="s">
+      <c r="AG1" s="24" t="s">
         <v>164</v>
       </c>
-      <c r="AH1" s="28" t="s">
+      <c r="AH1" s="25" t="s">
         <v>165</v>
       </c>
-      <c r="AI1" s="27" t="s">
+      <c r="AI1" s="24" t="s">
         <v>166</v>
       </c>
-      <c r="AJ1" s="28" t="s">
+      <c r="AJ1" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="AK1" s="27" t="s">
+      <c r="AK1" s="24" t="s">
         <v>168</v>
       </c>
-      <c r="AL1" s="29"/>
+      <c r="AL1" s="26"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="AA2" s="19" t="s">
+      <c r="AA2" s="17" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="N3" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="P3" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="T3" s="13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:38" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="20"/>
-      <c r="R4" s="14"/>
-      <c r="S4" s="20"/>
-      <c r="T4" s="14"/>
-      <c r="U4" s="20"/>
-      <c r="V4" s="14"/>
-      <c r="W4" s="20"/>
-      <c r="X4" s="14"/>
-      <c r="Y4" s="20"/>
-      <c r="Z4" s="14"/>
-      <c r="AA4" s="20"/>
-      <c r="AB4" s="14"/>
-      <c r="AC4" s="20"/>
-      <c r="AD4" s="14"/>
-      <c r="AE4" s="20"/>
-      <c r="AF4" s="14"/>
-      <c r="AG4" s="20"/>
-      <c r="AH4" s="14"/>
-      <c r="AI4" s="20"/>
-      <c r="AJ4" s="14"/>
-      <c r="AK4" s="20"/>
+      <c r="N3" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="P3" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="T3" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C4" s="18"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="18"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="18"/>
+      <c r="V4" s="12"/>
+      <c r="W4" s="18"/>
+      <c r="X4" s="12"/>
+      <c r="Y4" s="18"/>
+      <c r="Z4" s="12"/>
+      <c r="AA4" s="18"/>
+      <c r="AB4" s="12"/>
+      <c r="AC4" s="18"/>
+      <c r="AD4" s="12"/>
+      <c r="AE4" s="18"/>
+      <c r="AF4" s="12"/>
+      <c r="AG4" s="18"/>
+      <c r="AH4" s="12"/>
+      <c r="AI4" s="18"/>
+      <c r="AJ4" s="12"/>
+      <c r="AK4" s="18"/>
     </row>
     <row r="5" spans="1:38" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="15"/>
-      <c r="S5" s="21"/>
-      <c r="T5" s="15"/>
-      <c r="U5" s="21"/>
-      <c r="V5" s="15"/>
-      <c r="W5" s="21"/>
-      <c r="X5" s="15"/>
-      <c r="Y5" s="21"/>
-      <c r="Z5" s="15"/>
-      <c r="AA5" s="21"/>
-      <c r="AB5" s="15"/>
-      <c r="AC5" s="21"/>
-      <c r="AD5" s="15"/>
-      <c r="AE5" s="21"/>
-      <c r="AF5" s="15"/>
-      <c r="AG5" s="21"/>
-      <c r="AH5" s="15"/>
-      <c r="AI5" s="21"/>
-      <c r="AJ5" s="15"/>
-      <c r="AK5" s="21"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="19"/>
+      <c r="T5" s="13"/>
+      <c r="U5" s="19"/>
+      <c r="V5" s="13"/>
+      <c r="W5" s="19"/>
+      <c r="X5" s="13"/>
+      <c r="Y5" s="19"/>
+      <c r="Z5" s="13"/>
+      <c r="AA5" s="19"/>
+      <c r="AB5" s="13"/>
+      <c r="AC5" s="19"/>
+      <c r="AD5" s="13"/>
+      <c r="AE5" s="19"/>
+      <c r="AF5" s="13"/>
+      <c r="AG5" s="19"/>
+      <c r="AH5" s="13"/>
+      <c r="AI5" s="19"/>
+      <c r="AJ5" s="13"/>
+      <c r="AK5" s="19"/>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="L6" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="M6" s="22"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="22"/>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="22"/>
-      <c r="R6" s="16"/>
-      <c r="S6" s="22"/>
-      <c r="T6" s="16"/>
-      <c r="U6" s="22"/>
-      <c r="V6" s="16"/>
-      <c r="W6" s="22"/>
-      <c r="X6" s="16"/>
-      <c r="Y6" s="22"/>
-      <c r="Z6" s="16"/>
-      <c r="AA6" s="22"/>
-      <c r="AB6" s="16"/>
-      <c r="AC6" s="22"/>
-      <c r="AD6" s="16"/>
-      <c r="AE6" s="22"/>
-      <c r="AF6" s="16"/>
-      <c r="AG6" s="22"/>
-      <c r="AH6" s="16"/>
-      <c r="AI6" s="22"/>
-      <c r="AJ6" s="16"/>
-      <c r="AK6" s="22" t="s">
+      <c r="C6" s="20"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" s="20"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="20"/>
+      <c r="T6" s="14"/>
+      <c r="U6" s="20"/>
+      <c r="V6" s="14"/>
+      <c r="W6" s="20"/>
+      <c r="X6" s="14"/>
+      <c r="Y6" s="20"/>
+      <c r="Z6" s="14"/>
+      <c r="AA6" s="20"/>
+      <c r="AB6" s="14"/>
+      <c r="AC6" s="20"/>
+      <c r="AD6" s="14"/>
+      <c r="AE6" s="20"/>
+      <c r="AF6" s="14"/>
+      <c r="AG6" s="20"/>
+      <c r="AH6" s="14"/>
+      <c r="AI6" s="20"/>
+      <c r="AJ6" s="14"/>
+      <c r="AK6" s="20" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="23"/>
-      <c r="R7" s="17"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="17"/>
-      <c r="U7" s="23"/>
-      <c r="V7" s="17"/>
-      <c r="W7" s="23"/>
-      <c r="X7" s="17"/>
-      <c r="Y7" s="23"/>
-      <c r="Z7" s="17"/>
-      <c r="AA7" s="23"/>
-      <c r="AB7" s="17"/>
-      <c r="AC7" s="23"/>
-      <c r="AD7" s="17"/>
-      <c r="AE7" s="23"/>
-      <c r="AF7" s="17"/>
-      <c r="AG7" s="23"/>
-      <c r="AH7" s="17"/>
-      <c r="AI7" s="23"/>
-      <c r="AJ7" s="17"/>
-      <c r="AK7" s="23"/>
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="21"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="21"/>
+      <c r="T7" s="15"/>
+      <c r="U7" s="21"/>
+      <c r="V7" s="15"/>
+      <c r="W7" s="21"/>
+      <c r="X7" s="15"/>
+      <c r="Y7" s="21"/>
+      <c r="Z7" s="15"/>
+      <c r="AA7" s="21"/>
+      <c r="AB7" s="15"/>
+      <c r="AC7" s="21"/>
+      <c r="AD7" s="15"/>
+      <c r="AE7" s="21"/>
+      <c r="AF7" s="15"/>
+      <c r="AG7" s="21"/>
+      <c r="AH7" s="15"/>
+      <c r="AI7" s="21"/>
+      <c r="AJ7" s="15"/>
+      <c r="AK7" s="21"/>
     </row>
     <row r="8" spans="1:38" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="21"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="21"/>
-      <c r="R8" s="15"/>
-      <c r="S8" s="21"/>
-      <c r="T8" s="15"/>
-      <c r="U8" s="21"/>
-      <c r="V8" s="15"/>
-      <c r="W8" s="21"/>
-      <c r="X8" s="15"/>
-      <c r="Y8" s="21"/>
-      <c r="Z8" s="15"/>
-      <c r="AA8" s="21"/>
-      <c r="AB8" s="15"/>
-      <c r="AC8" s="21"/>
-      <c r="AD8" s="15"/>
-      <c r="AE8" s="21"/>
-      <c r="AF8" s="15"/>
-      <c r="AG8" s="21"/>
-      <c r="AH8" s="15"/>
-      <c r="AI8" s="21"/>
-      <c r="AJ8" s="15"/>
-      <c r="AK8" s="21"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="19"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="19"/>
+      <c r="V8" s="13"/>
+      <c r="W8" s="19"/>
+      <c r="X8" s="13"/>
+      <c r="Y8" s="19"/>
+      <c r="Z8" s="13"/>
+      <c r="AA8" s="19"/>
+      <c r="AB8" s="13"/>
+      <c r="AC8" s="19"/>
+      <c r="AD8" s="13"/>
+      <c r="AE8" s="19"/>
+      <c r="AF8" s="13"/>
+      <c r="AG8" s="19"/>
+      <c r="AH8" s="13"/>
+      <c r="AI8" s="19"/>
+      <c r="AJ8" s="13"/>
+      <c r="AK8" s="19"/>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="C9" s="22"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="22"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="22"/>
-      <c r="R9" s="16"/>
-      <c r="S9" s="22"/>
-      <c r="T9" s="16"/>
-      <c r="U9" s="22"/>
-      <c r="V9" s="16"/>
-      <c r="W9" s="22"/>
-      <c r="X9" s="16"/>
-      <c r="Y9" s="22"/>
-      <c r="Z9" s="16"/>
-      <c r="AA9" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="AB9" s="16"/>
-      <c r="AC9" s="22"/>
-      <c r="AD9" s="16"/>
-      <c r="AE9" s="22"/>
-      <c r="AF9" s="16"/>
-      <c r="AG9" s="22"/>
-      <c r="AH9" s="16"/>
-      <c r="AI9" s="22"/>
-      <c r="AJ9" s="16"/>
-      <c r="AK9" s="22"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="20"/>
+      <c r="T9" s="14"/>
+      <c r="U9" s="20"/>
+      <c r="V9" s="14"/>
+      <c r="W9" s="20"/>
+      <c r="X9" s="14"/>
+      <c r="Y9" s="20"/>
+      <c r="Z9" s="14"/>
+      <c r="AA9" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB9" s="14"/>
+      <c r="AC9" s="20"/>
+      <c r="AD9" s="14"/>
+      <c r="AE9" s="20"/>
+      <c r="AF9" s="14"/>
+      <c r="AG9" s="20"/>
+      <c r="AH9" s="14"/>
+      <c r="AI9" s="20"/>
+      <c r="AJ9" s="14"/>
+      <c r="AK9" s="20"/>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="J10" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="P10" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="T10" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="AK10" s="19" t="s">
+      <c r="J10" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="P10" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="T10" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="AK10" s="17" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="23"/>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="23"/>
-      <c r="R11" s="17"/>
-      <c r="S11" s="23"/>
-      <c r="T11" s="17"/>
-      <c r="U11" s="23"/>
-      <c r="V11" s="17"/>
-      <c r="W11" s="23"/>
-      <c r="X11" s="17"/>
-      <c r="Y11" s="23"/>
-      <c r="Z11" s="17"/>
-      <c r="AA11" s="23"/>
-      <c r="AB11" s="17"/>
-      <c r="AC11" s="23"/>
-      <c r="AD11" s="17"/>
-      <c r="AE11" s="23"/>
-      <c r="AF11" s="17"/>
-      <c r="AG11" s="23"/>
-      <c r="AH11" s="17"/>
-      <c r="AI11" s="23"/>
-      <c r="AJ11" s="17"/>
-      <c r="AK11" s="23"/>
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="21"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="21"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="21"/>
+      <c r="V11" s="15"/>
+      <c r="W11" s="21"/>
+      <c r="X11" s="15"/>
+      <c r="Y11" s="21"/>
+      <c r="Z11" s="15"/>
+      <c r="AA11" s="21"/>
+      <c r="AB11" s="15"/>
+      <c r="AC11" s="21"/>
+      <c r="AD11" s="15"/>
+      <c r="AE11" s="21"/>
+      <c r="AF11" s="15"/>
+      <c r="AG11" s="21"/>
+      <c r="AH11" s="15"/>
+      <c r="AI11" s="21"/>
+      <c r="AJ11" s="15"/>
+      <c r="AK11" s="21"/>
     </row>
     <row r="12" spans="1:38" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="21"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="21"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="21"/>
-      <c r="R12" s="15"/>
-      <c r="S12" s="21"/>
-      <c r="T12" s="15"/>
-      <c r="U12" s="21"/>
-      <c r="V12" s="15"/>
-      <c r="W12" s="21"/>
-      <c r="X12" s="15"/>
-      <c r="Y12" s="21"/>
-      <c r="Z12" s="15"/>
-      <c r="AA12" s="21"/>
-      <c r="AB12" s="15"/>
-      <c r="AC12" s="21"/>
-      <c r="AD12" s="15"/>
-      <c r="AE12" s="21"/>
-      <c r="AF12" s="15"/>
-      <c r="AG12" s="21"/>
-      <c r="AH12" s="15"/>
-      <c r="AI12" s="21"/>
-      <c r="AJ12" s="15"/>
-      <c r="AK12" s="21"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="13"/>
+      <c r="S12" s="19"/>
+      <c r="T12" s="13"/>
+      <c r="U12" s="19"/>
+      <c r="V12" s="13"/>
+      <c r="W12" s="19"/>
+      <c r="X12" s="13"/>
+      <c r="Y12" s="19"/>
+      <c r="Z12" s="13"/>
+      <c r="AA12" s="19"/>
+      <c r="AB12" s="13"/>
+      <c r="AC12" s="19"/>
+      <c r="AD12" s="13"/>
+      <c r="AE12" s="19"/>
+      <c r="AF12" s="13"/>
+      <c r="AG12" s="19"/>
+      <c r="AH12" s="13"/>
+      <c r="AI12" s="19"/>
+      <c r="AJ12" s="13"/>
+      <c r="AK12" s="19"/>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="22"/>
-      <c r="N13" s="16"/>
-      <c r="O13" s="22"/>
-      <c r="P13" s="16"/>
-      <c r="Q13" s="22"/>
-      <c r="R13" s="16"/>
-      <c r="S13" s="22"/>
-      <c r="T13" s="16"/>
-      <c r="U13" s="22"/>
-      <c r="V13" s="16"/>
-      <c r="W13" s="22"/>
-      <c r="X13" s="16"/>
-      <c r="Y13" s="22"/>
-      <c r="Z13" s="16"/>
-      <c r="AA13" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="AB13" s="16"/>
-      <c r="AC13" s="22"/>
-      <c r="AD13" s="16"/>
-      <c r="AE13" s="22"/>
-      <c r="AF13" s="16"/>
-      <c r="AG13" s="22"/>
-      <c r="AH13" s="16"/>
-      <c r="AI13" s="22"/>
-      <c r="AJ13" s="16"/>
-      <c r="AK13" s="22"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="20"/>
+      <c r="R13" s="14"/>
+      <c r="S13" s="20"/>
+      <c r="T13" s="14"/>
+      <c r="U13" s="20"/>
+      <c r="V13" s="14"/>
+      <c r="W13" s="20"/>
+      <c r="X13" s="14"/>
+      <c r="Y13" s="20"/>
+      <c r="Z13" s="14"/>
+      <c r="AA13" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB13" s="14"/>
+      <c r="AC13" s="20"/>
+      <c r="AD13" s="14"/>
+      <c r="AE13" s="20"/>
+      <c r="AF13" s="14"/>
+      <c r="AG13" s="20"/>
+      <c r="AH13" s="14"/>
+      <c r="AI13" s="20"/>
+      <c r="AJ13" s="14"/>
+      <c r="AK13" s="20"/>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="G14" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="P14" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="T14" s="13" t="s">
+      <c r="G14" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="P14" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="T14" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="AA15" s="19" t="s">
+      <c r="AA15" s="17" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="D16" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="P16" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="T16" s="13" t="s">
+      <c r="D16" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="P16" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="T16" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="Y17" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z17" s="13" t="s">
+      <c r="Y17" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z17" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="J18" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="P18" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="AK18" s="19" t="s">
+      <c r="J18" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="P18" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="AK18" s="17" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="23"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="23"/>
-      <c r="N19" s="17"/>
-      <c r="O19" s="23"/>
-      <c r="P19" s="17"/>
-      <c r="Q19" s="23"/>
-      <c r="R19" s="17"/>
-      <c r="S19" s="23"/>
-      <c r="T19" s="17"/>
-      <c r="U19" s="23"/>
-      <c r="V19" s="17"/>
-      <c r="W19" s="23"/>
-      <c r="X19" s="17"/>
-      <c r="Y19" s="23"/>
-      <c r="Z19" s="17"/>
-      <c r="AA19" s="23"/>
-      <c r="AB19" s="17"/>
-      <c r="AC19" s="23"/>
-      <c r="AD19" s="17"/>
-      <c r="AE19" s="23"/>
-      <c r="AF19" s="17"/>
-      <c r="AG19" s="23"/>
-      <c r="AH19" s="17"/>
-      <c r="AI19" s="23"/>
-      <c r="AJ19" s="17"/>
-      <c r="AK19" s="23"/>
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="21"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="21"/>
+      <c r="R19" s="15"/>
+      <c r="S19" s="21"/>
+      <c r="T19" s="15"/>
+      <c r="U19" s="21"/>
+      <c r="V19" s="15"/>
+      <c r="W19" s="21"/>
+      <c r="X19" s="15"/>
+      <c r="Y19" s="21"/>
+      <c r="Z19" s="15"/>
+      <c r="AA19" s="21"/>
+      <c r="AB19" s="15"/>
+      <c r="AC19" s="21"/>
+      <c r="AD19" s="15"/>
+      <c r="AE19" s="21"/>
+      <c r="AF19" s="15"/>
+      <c r="AG19" s="21"/>
+      <c r="AH19" s="15"/>
+      <c r="AI19" s="21"/>
+      <c r="AJ19" s="15"/>
+      <c r="AK19" s="21"/>
     </row>
     <row r="20" spans="1:37" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="21"/>
-      <c r="P20" s="15"/>
-      <c r="Q20" s="21"/>
-      <c r="R20" s="15"/>
-      <c r="S20" s="21"/>
-      <c r="T20" s="15"/>
-      <c r="U20" s="21"/>
-      <c r="V20" s="15"/>
-      <c r="W20" s="21"/>
-      <c r="X20" s="15"/>
-      <c r="Y20" s="21"/>
-      <c r="Z20" s="15"/>
-      <c r="AA20" s="21"/>
-      <c r="AB20" s="15"/>
-      <c r="AC20" s="21"/>
-      <c r="AD20" s="15"/>
-      <c r="AE20" s="21"/>
-      <c r="AF20" s="15"/>
-      <c r="AG20" s="21"/>
-      <c r="AH20" s="15"/>
-      <c r="AI20" s="21"/>
-      <c r="AJ20" s="15"/>
-      <c r="AK20" s="21"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="19"/>
+      <c r="R20" s="13"/>
+      <c r="S20" s="19"/>
+      <c r="T20" s="13"/>
+      <c r="U20" s="19"/>
+      <c r="V20" s="13"/>
+      <c r="W20" s="19"/>
+      <c r="X20" s="13"/>
+      <c r="Y20" s="19"/>
+      <c r="Z20" s="13"/>
+      <c r="AA20" s="19"/>
+      <c r="AB20" s="13"/>
+      <c r="AC20" s="19"/>
+      <c r="AD20" s="13"/>
+      <c r="AE20" s="19"/>
+      <c r="AF20" s="13"/>
+      <c r="AG20" s="19"/>
+      <c r="AH20" s="13"/>
+      <c r="AI20" s="19"/>
+      <c r="AJ20" s="13"/>
+      <c r="AK20" s="19"/>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="C21" s="22"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="22"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="22"/>
-      <c r="N21" s="16"/>
-      <c r="O21" s="22"/>
-      <c r="P21" s="16"/>
-      <c r="Q21" s="22"/>
-      <c r="R21" s="16"/>
-      <c r="S21" s="22"/>
-      <c r="T21" s="16"/>
-      <c r="U21" s="22"/>
-      <c r="V21" s="16"/>
-      <c r="W21" s="22"/>
-      <c r="X21" s="16"/>
-      <c r="Y21" s="22"/>
-      <c r="Z21" s="16"/>
-      <c r="AA21" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="AB21" s="16"/>
-      <c r="AC21" s="22"/>
-      <c r="AD21" s="16"/>
-      <c r="AE21" s="22"/>
-      <c r="AF21" s="16"/>
-      <c r="AG21" s="22"/>
-      <c r="AH21" s="16"/>
-      <c r="AI21" s="22"/>
-      <c r="AJ21" s="16"/>
-      <c r="AK21" s="22"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="20"/>
+      <c r="P21" s="14"/>
+      <c r="Q21" s="20"/>
+      <c r="R21" s="14"/>
+      <c r="S21" s="20"/>
+      <c r="T21" s="14"/>
+      <c r="U21" s="20"/>
+      <c r="V21" s="14"/>
+      <c r="W21" s="20"/>
+      <c r="X21" s="14"/>
+      <c r="Y21" s="20"/>
+      <c r="Z21" s="14"/>
+      <c r="AA21" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB21" s="14"/>
+      <c r="AC21" s="20"/>
+      <c r="AD21" s="14"/>
+      <c r="AE21" s="20"/>
+      <c r="AF21" s="14"/>
+      <c r="AG21" s="20"/>
+      <c r="AH21" s="14"/>
+      <c r="AI21" s="20"/>
+      <c r="AJ21" s="14"/>
+      <c r="AK21" s="20"/>
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="G22" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="P22" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="T22" s="13" t="s">
+      <c r="G22" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="P22" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="T22" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="AA23" s="19" t="s">
+      <c r="AA23" s="17" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="D24" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="P24" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="T24" s="13" t="s">
+      <c r="D24" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="P24" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="T24" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="Y25" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z25" s="13" t="s">
+      <c r="Y25" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z25" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="K26" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="O26" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="AK26" s="19" t="s">
+      <c r="K26" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="O26" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="AK26" s="17" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A27" s="9"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="17"/>
-      <c r="K27" s="23"/>
-      <c r="L27" s="17"/>
-      <c r="M27" s="23"/>
-      <c r="N27" s="17"/>
-      <c r="O27" s="23"/>
-      <c r="P27" s="17"/>
-      <c r="Q27" s="23"/>
-      <c r="R27" s="17"/>
-      <c r="S27" s="23"/>
-      <c r="T27" s="17"/>
-      <c r="U27" s="23"/>
-      <c r="V27" s="17"/>
-      <c r="W27" s="23"/>
-      <c r="X27" s="17"/>
-      <c r="Y27" s="23"/>
-      <c r="Z27" s="17"/>
-      <c r="AA27" s="23"/>
-      <c r="AB27" s="17"/>
-      <c r="AC27" s="23"/>
-      <c r="AD27" s="17"/>
-      <c r="AE27" s="23"/>
-      <c r="AF27" s="17"/>
-      <c r="AG27" s="23"/>
-      <c r="AH27" s="17"/>
-      <c r="AI27" s="23"/>
-      <c r="AJ27" s="17"/>
-      <c r="AK27" s="23"/>
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="21"/>
+      <c r="L27" s="15"/>
+      <c r="M27" s="21"/>
+      <c r="N27" s="15"/>
+      <c r="O27" s="21"/>
+      <c r="P27" s="15"/>
+      <c r="Q27" s="21"/>
+      <c r="R27" s="15"/>
+      <c r="S27" s="21"/>
+      <c r="T27" s="15"/>
+      <c r="U27" s="21"/>
+      <c r="V27" s="15"/>
+      <c r="W27" s="21"/>
+      <c r="X27" s="15"/>
+      <c r="Y27" s="21"/>
+      <c r="Z27" s="15"/>
+      <c r="AA27" s="21"/>
+      <c r="AB27" s="15"/>
+      <c r="AC27" s="21"/>
+      <c r="AD27" s="15"/>
+      <c r="AE27" s="21"/>
+      <c r="AF27" s="15"/>
+      <c r="AG27" s="21"/>
+      <c r="AH27" s="15"/>
+      <c r="AI27" s="21"/>
+      <c r="AJ27" s="15"/>
+      <c r="AK27" s="21"/>
     </row>
     <row r="28" spans="1:37" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="12"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="21"/>
-      <c r="J28" s="15"/>
-      <c r="K28" s="21"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="21"/>
-      <c r="N28" s="15"/>
-      <c r="O28" s="21"/>
-      <c r="P28" s="15"/>
-      <c r="Q28" s="21"/>
-      <c r="R28" s="15"/>
-      <c r="S28" s="21"/>
-      <c r="T28" s="15"/>
-      <c r="U28" s="21"/>
-      <c r="V28" s="15"/>
-      <c r="W28" s="21"/>
-      <c r="X28" s="15"/>
-      <c r="Y28" s="21"/>
-      <c r="Z28" s="15"/>
-      <c r="AA28" s="21"/>
-      <c r="AB28" s="15"/>
-      <c r="AC28" s="21"/>
-      <c r="AD28" s="15"/>
-      <c r="AE28" s="21"/>
-      <c r="AF28" s="15"/>
-      <c r="AG28" s="21"/>
-      <c r="AH28" s="15"/>
-      <c r="AI28" s="21"/>
-      <c r="AJ28" s="15"/>
-      <c r="AK28" s="21"/>
-    </row>
-    <row r="29" spans="1:37" s="36" customFormat="1" ht="24" x14ac:dyDescent="0.3">
-      <c r="A29" s="30" t="s">
+      <c r="B28" s="10"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="19"/>
+      <c r="P28" s="13"/>
+      <c r="Q28" s="19"/>
+      <c r="R28" s="13"/>
+      <c r="S28" s="19"/>
+      <c r="T28" s="13"/>
+      <c r="U28" s="19"/>
+      <c r="V28" s="13"/>
+      <c r="W28" s="19"/>
+      <c r="X28" s="13"/>
+      <c r="Y28" s="19"/>
+      <c r="Z28" s="13"/>
+      <c r="AA28" s="19"/>
+      <c r="AB28" s="13"/>
+      <c r="AC28" s="19"/>
+      <c r="AD28" s="13"/>
+      <c r="AE28" s="19"/>
+      <c r="AF28" s="13"/>
+      <c r="AG28" s="19"/>
+      <c r="AH28" s="13"/>
+      <c r="AI28" s="19"/>
+      <c r="AJ28" s="13"/>
+      <c r="AK28" s="19"/>
+    </row>
+    <row r="29" spans="1:37" s="33" customFormat="1" ht="24" x14ac:dyDescent="0.3">
+      <c r="A29" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="B29" s="31" t="s">
+      <c r="B29" s="28" t="s">
         <v>171</v>
       </c>
-      <c r="C29" s="32"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="33"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="K29" s="32"/>
-      <c r="L29" s="33"/>
-      <c r="M29" s="32"/>
-      <c r="N29" s="33"/>
-      <c r="O29" s="32"/>
-      <c r="P29" s="33"/>
-      <c r="Q29" s="32"/>
-      <c r="R29" s="33"/>
-      <c r="S29" s="32"/>
-      <c r="T29" s="33"/>
-      <c r="U29" s="32"/>
-      <c r="V29" s="33"/>
-      <c r="W29" s="32"/>
-      <c r="X29" s="33"/>
-      <c r="Y29" s="32"/>
-      <c r="Z29" s="33"/>
-      <c r="AA29" s="32"/>
-      <c r="AB29" s="33"/>
-      <c r="AC29" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="AD29" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="AE29" s="35" t="s">
-        <v>19</v>
-      </c>
-      <c r="AF29" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="AG29" s="35" t="s">
-        <v>19</v>
-      </c>
-      <c r="AH29" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="AI29" s="32"/>
-      <c r="AJ29" s="33"/>
-      <c r="AK29" s="32" t="s">
+      <c r="C29" s="29"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="K29" s="29"/>
+      <c r="L29" s="30"/>
+      <c r="M29" s="29"/>
+      <c r="N29" s="30"/>
+      <c r="O29" s="29"/>
+      <c r="P29" s="30"/>
+      <c r="Q29" s="29"/>
+      <c r="R29" s="30"/>
+      <c r="S29" s="29"/>
+      <c r="T29" s="30"/>
+      <c r="U29" s="29"/>
+      <c r="V29" s="30"/>
+      <c r="W29" s="29"/>
+      <c r="X29" s="30"/>
+      <c r="Y29" s="29"/>
+      <c r="Z29" s="30"/>
+      <c r="AA29" s="29"/>
+      <c r="AB29" s="30"/>
+      <c r="AC29" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD29" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE29" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF29" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="AG29" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH29" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="AI29" s="29"/>
+      <c r="AJ29" s="30"/>
+      <c r="AK29" s="29" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A30" s="9"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="17"/>
-      <c r="K30" s="23"/>
-      <c r="L30" s="17"/>
-      <c r="M30" s="23"/>
-      <c r="N30" s="17"/>
-      <c r="O30" s="23"/>
-      <c r="P30" s="17"/>
-      <c r="Q30" s="23"/>
-      <c r="R30" s="17"/>
-      <c r="S30" s="23"/>
-      <c r="T30" s="17"/>
-      <c r="U30" s="23"/>
-      <c r="V30" s="17"/>
-      <c r="W30" s="23"/>
-      <c r="X30" s="17"/>
-      <c r="Y30" s="23"/>
-      <c r="Z30" s="17"/>
-      <c r="AA30" s="23"/>
-      <c r="AB30" s="17"/>
-      <c r="AC30" s="23"/>
-      <c r="AD30" s="17"/>
-      <c r="AE30" s="23"/>
-      <c r="AF30" s="17"/>
-      <c r="AG30" s="23"/>
-      <c r="AH30" s="17"/>
-      <c r="AI30" s="23"/>
-      <c r="AJ30" s="17"/>
-      <c r="AK30" s="23"/>
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="21"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="21"/>
+      <c r="P30" s="15"/>
+      <c r="Q30" s="21"/>
+      <c r="R30" s="15"/>
+      <c r="S30" s="21"/>
+      <c r="T30" s="15"/>
+      <c r="U30" s="21"/>
+      <c r="V30" s="15"/>
+      <c r="W30" s="21"/>
+      <c r="X30" s="15"/>
+      <c r="Y30" s="21"/>
+      <c r="Z30" s="15"/>
+      <c r="AA30" s="21"/>
+      <c r="AB30" s="15"/>
+      <c r="AC30" s="21"/>
+      <c r="AD30" s="15"/>
+      <c r="AE30" s="21"/>
+      <c r="AF30" s="15"/>
+      <c r="AG30" s="21"/>
+      <c r="AH30" s="15"/>
+      <c r="AI30" s="21"/>
+      <c r="AJ30" s="15"/>
+      <c r="AK30" s="21"/>
     </row>
     <row r="31" spans="1:37" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B31" s="12"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="15"/>
-      <c r="I31" s="21"/>
-      <c r="J31" s="15"/>
-      <c r="K31" s="21"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="21"/>
-      <c r="N31" s="15"/>
-      <c r="O31" s="21"/>
-      <c r="P31" s="15"/>
-      <c r="Q31" s="21"/>
-      <c r="R31" s="15"/>
-      <c r="S31" s="21"/>
-      <c r="T31" s="15"/>
-      <c r="U31" s="21"/>
-      <c r="V31" s="15"/>
-      <c r="W31" s="21"/>
-      <c r="X31" s="15"/>
-      <c r="Y31" s="21"/>
-      <c r="Z31" s="15"/>
-      <c r="AA31" s="21"/>
-      <c r="AB31" s="15"/>
-      <c r="AC31" s="21"/>
-      <c r="AD31" s="15"/>
-      <c r="AE31" s="21"/>
-      <c r="AF31" s="15"/>
-      <c r="AG31" s="21"/>
-      <c r="AH31" s="15"/>
-      <c r="AI31" s="21"/>
-      <c r="AJ31" s="15"/>
-      <c r="AK31" s="21"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="13"/>
+      <c r="O31" s="19"/>
+      <c r="P31" s="13"/>
+      <c r="Q31" s="19"/>
+      <c r="R31" s="13"/>
+      <c r="S31" s="19"/>
+      <c r="T31" s="13"/>
+      <c r="U31" s="19"/>
+      <c r="V31" s="13"/>
+      <c r="W31" s="19"/>
+      <c r="X31" s="13"/>
+      <c r="Y31" s="19"/>
+      <c r="Z31" s="13"/>
+      <c r="AA31" s="19"/>
+      <c r="AB31" s="13"/>
+      <c r="AC31" s="19"/>
+      <c r="AD31" s="13"/>
+      <c r="AE31" s="19"/>
+      <c r="AF31" s="13"/>
+      <c r="AG31" s="19"/>
+      <c r="AH31" s="13"/>
+      <c r="AI31" s="19"/>
+      <c r="AJ31" s="13"/>
+      <c r="AK31" s="19"/>
     </row>
     <row r="32" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
+      <c r="A32" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B32" s="25" t="s">
+      <c r="B32" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="C32" s="24"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="24"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="24"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="24"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="24"/>
-      <c r="L32" s="18"/>
-      <c r="M32" s="24"/>
-      <c r="N32" s="18"/>
-      <c r="O32" s="24"/>
-      <c r="P32" s="18"/>
-      <c r="Q32" s="24"/>
-      <c r="R32" s="18"/>
-      <c r="S32" s="24"/>
-      <c r="T32" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="U32" s="24"/>
-      <c r="V32" s="18"/>
-      <c r="W32" s="24"/>
-      <c r="X32" s="18"/>
-      <c r="Y32" s="24"/>
-      <c r="Z32" s="18"/>
-      <c r="AA32" s="24"/>
-      <c r="AB32" s="18"/>
-      <c r="AC32" s="24"/>
-      <c r="AD32" s="18"/>
-      <c r="AE32" s="24"/>
-      <c r="AF32" s="18"/>
-      <c r="AG32" s="24"/>
-      <c r="AH32" s="18"/>
-      <c r="AI32" s="24"/>
-      <c r="AJ32" s="18"/>
-      <c r="AK32" s="24"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="22"/>
+      <c r="J32" s="16"/>
+      <c r="K32" s="22"/>
+      <c r="L32" s="16"/>
+      <c r="M32" s="22"/>
+      <c r="N32" s="16"/>
+      <c r="O32" s="22"/>
+      <c r="P32" s="16"/>
+      <c r="Q32" s="22"/>
+      <c r="R32" s="16"/>
+      <c r="S32" s="22"/>
+      <c r="T32" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="U32" s="22"/>
+      <c r="V32" s="16"/>
+      <c r="W32" s="22"/>
+      <c r="X32" s="16"/>
+      <c r="Y32" s="22"/>
+      <c r="Z32" s="16"/>
+      <c r="AA32" s="22"/>
+      <c r="AB32" s="16"/>
+      <c r="AC32" s="22"/>
+      <c r="AD32" s="16"/>
+      <c r="AE32" s="22"/>
+      <c r="AF32" s="16"/>
+      <c r="AG32" s="22"/>
+      <c r="AH32" s="16"/>
+      <c r="AI32" s="22"/>
+      <c r="AJ32" s="16"/>
+      <c r="AK32" s="22"/>
     </row>
     <row r="33" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="C33" s="22"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="16"/>
-      <c r="I33" s="22"/>
-      <c r="J33" s="16"/>
-      <c r="K33" s="22"/>
-      <c r="L33" s="16"/>
-      <c r="M33" s="22"/>
-      <c r="N33" s="16"/>
-      <c r="O33" s="22"/>
-      <c r="P33" s="16"/>
-      <c r="Q33" s="22"/>
-      <c r="R33" s="16"/>
-      <c r="S33" s="22"/>
-      <c r="T33" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="U33" s="22"/>
-      <c r="V33" s="16"/>
-      <c r="W33" s="22"/>
-      <c r="X33" s="16"/>
-      <c r="Y33" s="22"/>
-      <c r="Z33" s="16"/>
-      <c r="AA33" s="22"/>
-      <c r="AB33" s="16"/>
-      <c r="AC33" s="22"/>
-      <c r="AD33" s="16"/>
-      <c r="AE33" s="22"/>
-      <c r="AF33" s="16"/>
-      <c r="AG33" s="22"/>
-      <c r="AH33" s="16"/>
-      <c r="AI33" s="22"/>
-      <c r="AJ33" s="16"/>
-      <c r="AK33" s="22"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="20"/>
+      <c r="L33" s="14"/>
+      <c r="M33" s="20"/>
+      <c r="N33" s="14"/>
+      <c r="O33" s="20"/>
+      <c r="P33" s="14"/>
+      <c r="Q33" s="20"/>
+      <c r="R33" s="14"/>
+      <c r="S33" s="20"/>
+      <c r="T33" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="U33" s="20"/>
+      <c r="V33" s="14"/>
+      <c r="W33" s="20"/>
+      <c r="X33" s="14"/>
+      <c r="Y33" s="20"/>
+      <c r="Z33" s="14"/>
+      <c r="AA33" s="20"/>
+      <c r="AB33" s="14"/>
+      <c r="AC33" s="20"/>
+      <c r="AD33" s="14"/>
+      <c r="AE33" s="20"/>
+      <c r="AF33" s="14"/>
+      <c r="AG33" s="20"/>
+      <c r="AH33" s="14"/>
+      <c r="AI33" s="20"/>
+      <c r="AJ33" s="14"/>
+      <c r="AK33" s="20"/>
     </row>
     <row r="34" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="C34" s="22"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="G34" s="22"/>
-      <c r="H34" s="16"/>
-      <c r="I34" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="J34" s="16"/>
-      <c r="K34" s="22"/>
-      <c r="L34" s="16"/>
-      <c r="M34" s="22"/>
-      <c r="N34" s="16"/>
-      <c r="O34" s="22"/>
-      <c r="P34" s="16"/>
-      <c r="Q34" s="22"/>
-      <c r="R34" s="16"/>
-      <c r="S34" s="22"/>
-      <c r="T34" s="16"/>
-      <c r="U34" s="22"/>
-      <c r="V34" s="16"/>
-      <c r="W34" s="22"/>
-      <c r="X34" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y34" s="22"/>
-      <c r="Z34" s="16"/>
-      <c r="AA34" s="22"/>
-      <c r="AB34" s="16"/>
-      <c r="AC34" s="22"/>
-      <c r="AD34" s="16"/>
-      <c r="AE34" s="22"/>
-      <c r="AF34" s="16"/>
-      <c r="AG34" s="22"/>
-      <c r="AH34" s="16"/>
-      <c r="AI34" s="22"/>
-      <c r="AJ34" s="16"/>
-      <c r="AK34" s="22"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G34" s="20"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="J34" s="14"/>
+      <c r="K34" s="20"/>
+      <c r="L34" s="14"/>
+      <c r="M34" s="20"/>
+      <c r="N34" s="14"/>
+      <c r="O34" s="20"/>
+      <c r="P34" s="14"/>
+      <c r="Q34" s="20"/>
+      <c r="R34" s="14"/>
+      <c r="S34" s="20"/>
+      <c r="T34" s="14"/>
+      <c r="U34" s="20"/>
+      <c r="V34" s="14"/>
+      <c r="W34" s="20"/>
+      <c r="X34" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y34" s="20"/>
+      <c r="Z34" s="14"/>
+      <c r="AA34" s="20"/>
+      <c r="AB34" s="14"/>
+      <c r="AC34" s="20"/>
+      <c r="AD34" s="14"/>
+      <c r="AE34" s="20"/>
+      <c r="AF34" s="14"/>
+      <c r="AG34" s="20"/>
+      <c r="AH34" s="14"/>
+      <c r="AI34" s="20"/>
+      <c r="AJ34" s="14"/>
+      <c r="AK34" s="20"/>
     </row>
     <row r="35" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="AB35" s="13" t="s">
+      <c r="AB35" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="36" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
+      <c r="A36" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="H36" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="O36" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="X36" s="13" t="s">
+      <c r="H36" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="O36" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="X36" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="AB37" s="13" t="s">
+      <c r="AB37" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
+      <c r="A38" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="S38" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="AA38" s="19" t="s">
+      <c r="S38" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA38" s="17" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="39" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
+      <c r="A39" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="S39" s="19" t="s">
+      <c r="S39" s="17" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="40" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
+      <c r="A40" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="AA40" s="19" t="s">
+      <c r="AA40" s="17" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="41" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
+      <c r="A41" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="G41" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="P41" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="T41" s="13" t="s">
+      <c r="G41" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="P41" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="T41" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="42" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
+      <c r="A42" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B42" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="AA42" s="19" t="s">
+      <c r="AA42" s="17" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="43" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="D43" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="P43" s="13" t="s">
+      <c r="D43" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="P43" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="44" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A44" s="7" t="s">
+      <c r="A44" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="U44" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="V44" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="AK44" s="19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="45" spans="1:37" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="9"/>
-      <c r="B45" s="9"/>
-      <c r="C45" s="23"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="23"/>
-      <c r="F45" s="17"/>
-      <c r="G45" s="23"/>
-      <c r="H45" s="17"/>
-      <c r="I45" s="23"/>
-      <c r="J45" s="17"/>
-      <c r="K45" s="23"/>
-      <c r="L45" s="17"/>
-      <c r="M45" s="23"/>
-      <c r="N45" s="17"/>
-      <c r="O45" s="23"/>
-      <c r="P45" s="17"/>
-      <c r="Q45" s="23"/>
-      <c r="R45" s="17"/>
-      <c r="S45" s="23"/>
-      <c r="T45" s="17"/>
-      <c r="U45" s="23"/>
-      <c r="V45" s="17"/>
-      <c r="W45" s="23"/>
-      <c r="X45" s="17"/>
-      <c r="Y45" s="23"/>
-      <c r="Z45" s="17"/>
-      <c r="AA45" s="23"/>
-      <c r="AB45" s="17"/>
-      <c r="AC45" s="23"/>
-      <c r="AD45" s="17"/>
-      <c r="AE45" s="23"/>
-      <c r="AF45" s="17"/>
-      <c r="AG45" s="23"/>
-      <c r="AH45" s="17"/>
-      <c r="AI45" s="23"/>
-      <c r="AJ45" s="17"/>
-      <c r="AK45" s="23"/>
+      <c r="U44" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="V44" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="AK44" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="45" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A45" s="8"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="15"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="15"/>
+      <c r="K45" s="21"/>
+      <c r="L45" s="15"/>
+      <c r="M45" s="21"/>
+      <c r="N45" s="15"/>
+      <c r="O45" s="21"/>
+      <c r="P45" s="15"/>
+      <c r="Q45" s="21"/>
+      <c r="R45" s="15"/>
+      <c r="S45" s="21"/>
+      <c r="T45" s="15"/>
+      <c r="U45" s="21"/>
+      <c r="V45" s="15"/>
+      <c r="W45" s="21"/>
+      <c r="X45" s="15"/>
+      <c r="Y45" s="21"/>
+      <c r="Z45" s="15"/>
+      <c r="AA45" s="21"/>
+      <c r="AB45" s="15"/>
+      <c r="AC45" s="21"/>
+      <c r="AD45" s="15"/>
+      <c r="AE45" s="21"/>
+      <c r="AF45" s="15"/>
+      <c r="AG45" s="21"/>
+      <c r="AH45" s="15"/>
+      <c r="AI45" s="21"/>
+      <c r="AJ45" s="15"/>
+      <c r="AK45" s="21"/>
     </row>
     <row r="46" spans="1:37" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B46" s="12"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="15"/>
-      <c r="E46" s="21"/>
-      <c r="F46" s="15"/>
-      <c r="G46" s="21"/>
-      <c r="H46" s="15"/>
-      <c r="I46" s="21"/>
-      <c r="J46" s="15"/>
-      <c r="K46" s="21"/>
-      <c r="L46" s="15"/>
-      <c r="M46" s="21"/>
-      <c r="N46" s="15"/>
-      <c r="O46" s="21"/>
-      <c r="P46" s="15"/>
-      <c r="Q46" s="21"/>
-      <c r="R46" s="15"/>
-      <c r="S46" s="21"/>
-      <c r="T46" s="15"/>
-      <c r="U46" s="21"/>
-      <c r="V46" s="15"/>
-      <c r="W46" s="21"/>
-      <c r="X46" s="15"/>
-      <c r="Y46" s="21"/>
-      <c r="Z46" s="15"/>
-      <c r="AA46" s="21"/>
-      <c r="AB46" s="15"/>
-      <c r="AC46" s="21"/>
-      <c r="AD46" s="15"/>
-      <c r="AE46" s="21"/>
-      <c r="AF46" s="15"/>
-      <c r="AG46" s="21"/>
-      <c r="AH46" s="15"/>
-      <c r="AI46" s="21"/>
-      <c r="AJ46" s="15"/>
-      <c r="AK46" s="21"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="19"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="19"/>
+      <c r="J46" s="13"/>
+      <c r="K46" s="19"/>
+      <c r="L46" s="13"/>
+      <c r="M46" s="19"/>
+      <c r="N46" s="13"/>
+      <c r="O46" s="19"/>
+      <c r="P46" s="13"/>
+      <c r="Q46" s="19"/>
+      <c r="R46" s="13"/>
+      <c r="S46" s="19"/>
+      <c r="T46" s="13"/>
+      <c r="U46" s="19"/>
+      <c r="V46" s="13"/>
+      <c r="W46" s="19"/>
+      <c r="X46" s="13"/>
+      <c r="Y46" s="19"/>
+      <c r="Z46" s="13"/>
+      <c r="AA46" s="19"/>
+      <c r="AB46" s="13"/>
+      <c r="AC46" s="19"/>
+      <c r="AD46" s="13"/>
+      <c r="AE46" s="19"/>
+      <c r="AF46" s="13"/>
+      <c r="AG46" s="19"/>
+      <c r="AH46" s="13"/>
+      <c r="AI46" s="19"/>
+      <c r="AJ46" s="13"/>
+      <c r="AK46" s="19"/>
     </row>
     <row r="47" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A47" s="8" t="s">
+      <c r="A47" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B47" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="C47" s="22"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="22"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="22"/>
-      <c r="H47" s="16"/>
-      <c r="I47" s="22"/>
-      <c r="J47" s="16"/>
-      <c r="K47" s="22"/>
-      <c r="L47" s="16"/>
-      <c r="M47" s="22"/>
-      <c r="N47" s="16"/>
-      <c r="O47" s="22"/>
-      <c r="P47" s="16"/>
-      <c r="Q47" s="22"/>
-      <c r="R47" s="16"/>
-      <c r="S47" s="22"/>
-      <c r="T47" s="16"/>
-      <c r="U47" s="22"/>
-      <c r="V47" s="16"/>
-      <c r="W47" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="X47" s="16"/>
-      <c r="Y47" s="22"/>
-      <c r="Z47" s="16"/>
-      <c r="AA47" s="22"/>
-      <c r="AB47" s="16"/>
-      <c r="AC47" s="22"/>
-      <c r="AD47" s="16"/>
-      <c r="AE47" s="22"/>
-      <c r="AF47" s="16"/>
-      <c r="AG47" s="22"/>
-      <c r="AH47" s="16"/>
-      <c r="AI47" s="22"/>
-      <c r="AJ47" s="16"/>
-      <c r="AK47" s="22"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="20"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="20"/>
+      <c r="J47" s="14"/>
+      <c r="K47" s="20"/>
+      <c r="L47" s="14"/>
+      <c r="M47" s="20"/>
+      <c r="N47" s="14"/>
+      <c r="O47" s="20"/>
+      <c r="P47" s="14"/>
+      <c r="Q47" s="20"/>
+      <c r="R47" s="14"/>
+      <c r="S47" s="20"/>
+      <c r="T47" s="14"/>
+      <c r="U47" s="20"/>
+      <c r="V47" s="14"/>
+      <c r="W47" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="X47" s="14"/>
+      <c r="Y47" s="20"/>
+      <c r="Z47" s="14"/>
+      <c r="AA47" s="20"/>
+      <c r="AB47" s="14"/>
+      <c r="AC47" s="20"/>
+      <c r="AD47" s="14"/>
+      <c r="AE47" s="20"/>
+      <c r="AF47" s="14"/>
+      <c r="AG47" s="20"/>
+      <c r="AH47" s="14"/>
+      <c r="AI47" s="20"/>
+      <c r="AJ47" s="14"/>
+      <c r="AK47" s="20"/>
     </row>
     <row r="48" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A48" s="7" t="s">
+      <c r="A48" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B48" s="7" t="s">
+      <c r="B48" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="AB48" s="13" t="s">
+      <c r="AB48" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="49" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A49" s="8" t="s">
+      <c r="A49" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="B49" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="D49" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="P49" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="W49" s="19" t="s">
+      <c r="D49" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="P49" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="W49" s="17" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="50" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A50" s="7" t="s">
+      <c r="A50" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B50" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="AB50" s="13" t="s">
+      <c r="AB50" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="51" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A51" s="8" t="s">
+      <c r="A51" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="B51" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="G51" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="P51" s="13" t="s">
+      <c r="G51" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="P51" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="52" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A52" s="7" t="s">
+      <c r="A52" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B52" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="U52" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="V52" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="AK52" s="19" t="s">
+      <c r="U52" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="V52" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="AK52" s="17" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="53" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A53" s="7"/>
-      <c r="B53" s="7"/>
+      <c r="A53" s="6"/>
+      <c r="B53" s="6"/>
     </row>
     <row r="54" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A54" s="7"/>
-      <c r="B54" s="7"/>
+      <c r="A54" s="6"/>
+      <c r="B54" s="6"/>
     </row>
     <row r="55" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A55" s="7"/>
-      <c r="B55" s="7"/>
+      <c r="A55" s="6"/>
+      <c r="B55" s="6"/>
     </row>
     <row r="56" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A56" s="7"/>
-      <c r="B56" s="7"/>
+      <c r="A56" s="6"/>
+      <c r="B56" s="6"/>
     </row>
     <row r="57" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A57" s="7"/>
-      <c r="B57" s="7"/>
+      <c r="A57" s="6"/>
+      <c r="B57" s="6"/>
     </row>
     <row r="58" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A58" s="7"/>
-      <c r="B58" s="7"/>
+      <c r="A58" s="6"/>
+      <c r="B58" s="6"/>
     </row>
     <row r="59" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A59" s="7"/>
-      <c r="B59" s="7"/>
+      <c r="A59" s="6"/>
+      <c r="B59" s="6"/>
     </row>
     <row r="60" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A60" s="7"/>
-      <c r="B60" s="7"/>
+      <c r="A60" s="6"/>
+      <c r="B60" s="6"/>
     </row>
     <row r="61" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A61" s="7"/>
-      <c r="B61" s="7"/>
+      <c r="A61" s="6"/>
+      <c r="B61" s="6"/>
     </row>
     <row r="62" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A62" s="7"/>
-      <c r="B62" s="7"/>
+      <c r="A62" s="6"/>
+      <c r="B62" s="6"/>
     </row>
     <row r="63" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A63" s="7"/>
-      <c r="B63" s="7"/>
+      <c r="A63" s="6"/>
+      <c r="B63" s="6"/>
     </row>
     <row r="64" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A64" s="7"/>
-      <c r="B64" s="7"/>
+      <c r="A64" s="6"/>
+      <c r="B64" s="6"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="7"/>
-      <c r="B65" s="7"/>
+      <c r="A65" s="6"/>
+      <c r="B65" s="6"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="7"/>
-      <c r="B66" s="7"/>
+      <c r="A66" s="6"/>
+      <c r="B66" s="6"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="7"/>
-      <c r="B67" s="7"/>
+      <c r="A67" s="6"/>
+      <c r="B67" s="6"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="7"/>
-      <c r="B68" s="7"/>
+      <c r="A68" s="6"/>
+      <c r="B68" s="6"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="7"/>
-      <c r="B69" s="7"/>
+      <c r="A69" s="6"/>
+      <c r="B69" s="6"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="7"/>
-      <c r="B70" s="7"/>
+      <c r="A70" s="6"/>
+      <c r="B70" s="6"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="7"/>
-      <c r="B71" s="7"/>
+      <c r="A71" s="6"/>
+      <c r="B71" s="6"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="7"/>
-      <c r="B72" s="7"/>
+      <c r="A72" s="6"/>
+      <c r="B72" s="6"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="7"/>
-      <c r="B73" s="7"/>
+      <c r="A73" s="6"/>
+      <c r="B73" s="6"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="7"/>
-      <c r="B74" s="7"/>
+      <c r="A74" s="6"/>
+      <c r="B74" s="6"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="7"/>
-      <c r="B75" s="7"/>
+      <c r="A75" s="6"/>
+      <c r="B75" s="6"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="7"/>
-      <c r="B76" s="7"/>
+      <c r="A76" s="6"/>
+      <c r="B76" s="6"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="7"/>
-      <c r="B77" s="7"/>
+      <c r="A77" s="6"/>
+      <c r="B77" s="6"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="7"/>
-      <c r="B78" s="7"/>
+      <c r="A78" s="6"/>
+      <c r="B78" s="6"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="7"/>
-      <c r="B79" s="7"/>
+      <c r="A79" s="6"/>
+      <c r="B79" s="6"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="7"/>
-      <c r="B80" s="7"/>
+      <c r="A80" s="6"/>
+      <c r="B80" s="6"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="7"/>
-      <c r="B81" s="7"/>
+      <c r="A81" s="6"/>
+      <c r="B81" s="6"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="7"/>
-      <c r="B82" s="7"/>
+      <c r="A82" s="6"/>
+      <c r="B82" s="6"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="7"/>
-      <c r="B83" s="7"/>
+      <c r="A83" s="6"/>
+      <c r="B83" s="6"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="7"/>
-      <c r="B84" s="7"/>
+      <c r="A84" s="6"/>
+      <c r="B84" s="6"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="7"/>
-      <c r="B85" s="7"/>
+      <c r="A85" s="6"/>
+      <c r="B85" s="6"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="7"/>
-      <c r="B86" s="7"/>
+      <c r="A86" s="6"/>
+      <c r="B86" s="6"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="9"/>
-      <c r="B87" s="9"/>
+      <c r="A87" s="8"/>
+      <c r="B87" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7656,10 +7695,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7669,7 +7708,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="34" t="s">
         <v>176</v>
       </c>
     </row>
@@ -7714,7 +7753,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="34" t="s">
         <v>268</v>
       </c>
     </row>
@@ -7735,37 +7774,82 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="38" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
+      <c r="B23" s="38"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="38"/>
+      <c r="B24" s="38" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="38"/>
+      <c r="B25" s="38" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="38"/>
+      <c r="B26" s="38" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="38"/>
+      <c r="B27" s="38" t="s">
         <v>278</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" s="39" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B34" s="34" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35" s="40" t="s">
+        <v>286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Work in progress on controller/sequencer
</commit_message>
<xml_diff>
--- a/Documentation/Instructions_T-States.xlsx
+++ b/Documentation/Instructions_T-States.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Projects\Active\TTL-Computer\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32ADC23-57D7-428A-8898-4D6A22D098E4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77968BE0-976D-45C8-91FC-18DA31A362F3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="289">
   <si>
     <t>Opcode</t>
   </si>
@@ -4529,6 +4529,12 @@
   </si>
   <si>
     <t>[unused][group][flags][instruction][t-state]</t>
+  </si>
+  <si>
+    <t>Stack</t>
+  </si>
+  <si>
+    <t>$FF00-$FFFF</t>
   </si>
 </sst>
 </file>
@@ -5148,7 +5154,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView topLeftCell="F31" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
@@ -6048,7 +6054,7 @@
     <col min="38" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" customFormat="1" ht="46.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:38" customFormat="1" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9"/>
       <c r="B1" s="9"/>
       <c r="C1" s="24" t="s">
@@ -7695,10 +7701,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7737,118 +7743,128 @@
         <v>181</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>287</v>
+      </c>
+    </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="34" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="34" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
         <v>271</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="38" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="38" t="s">
         <v>274</v>
       </c>
-      <c r="B23" s="38"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="38"/>
-      <c r="B24" s="38" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="38"/>
-      <c r="B25" s="38" t="s">
-        <v>276</v>
-      </c>
+      <c r="B25" s="38"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="38"/>
       <c r="B26" s="38" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="38"/>
       <c r="B27" s="38" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="38"/>
+      <c r="B28" s="38" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="38"/>
+      <c r="B29" s="38" t="s">
         <v>278</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B33" s="39" t="s">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35" s="39" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B34" s="34" t="s">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B36" s="34" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B35" s="40" t="s">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B37" s="40" t="s">
         <v>286</v>
       </c>
     </row>

</xml_diff>